<commit_message>
pcb and lab 7 report done
</commit_message>
<xml_diff>
--- a/deliverables/BOM.xlsx
+++ b/deliverables/BOM.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\EE345L Class\EE445LTeachingMaterials\0000_Spring2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Keil_v5\ValvanoWareTM4C123v5\ece-445l-lab-7-8-11-sp24-ps33536-hjs2235-shp695-wtc534\deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A28EEF-BE93-4159-9EEE-C41A6AAED890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBB6929-0533-4B78-9787-2768E9818840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="555" yWindow="1110" windowWidth="28740" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
     <sheet name="SurfaceMountParts" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="BOM" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Parts!$A$5:$J$36</definedName>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="634">
   <si>
     <t>Quantity</t>
   </si>
@@ -1672,12 +1672,382 @@
   <si>
     <t>https://www.allelectronics.com/item/shs-40/1-x-40-header-0.1-spacing/1.html</t>
   </si>
+  <si>
+    <t>Source:</t>
+  </si>
+  <si>
+    <t>C:\Keil_v5\ValvanoWareTM4C123v5\ece-445l-lab-7-8-11-sp24-ps33536-hjs2235-shp695-wtc534\hw\baseline_project\baseline_project.kicad_sch</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>Tool:</t>
+  </si>
+  <si>
+    <t>Eeschema 7.0.10</t>
+  </si>
+  <si>
+    <t>Generator:</t>
+  </si>
+  <si>
+    <t>C:\Program Files\KiCad\7.0\bin\scripting\plugins/bom_csv_grouped_by_value.py</t>
+  </si>
+  <si>
+    <t>Component Count:</t>
+  </si>
+  <si>
+    <t>Collated Components:</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Reference(s)</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>LibPart</t>
+  </si>
+  <si>
+    <t>Footprint</t>
+  </si>
+  <si>
+    <t>Datasheet</t>
+  </si>
+  <si>
+    <t>DNP</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>1uF</t>
+  </si>
+  <si>
+    <t>Device:C</t>
+  </si>
+  <si>
+    <t>ECE445L:C_Axial_200mil</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>Checkout</t>
+  </si>
+  <si>
+    <t>C2, C6, C7, C8, C9, C10, C11</t>
+  </si>
+  <si>
+    <t>0.1uF</t>
+  </si>
+  <si>
+    <t>ECE445L:C</t>
+  </si>
+  <si>
+    <t>C3, C4, C5</t>
+  </si>
+  <si>
+    <t>4.7uF</t>
+  </si>
+  <si>
+    <t>C101, C102</t>
+  </si>
+  <si>
+    <t>100nF</t>
+  </si>
+  <si>
+    <t>Device:C_Small</t>
+  </si>
+  <si>
+    <t>C103, C104</t>
+  </si>
+  <si>
+    <t>Device:C_Polarized_Small_US</t>
+  </si>
+  <si>
+    <t>ECE445L:CP_Radial_Tantal200mil</t>
+  </si>
+  <si>
+    <t>H1, H2, H3, H4</t>
+  </si>
+  <si>
+    <t>ECE445L:MountingHole</t>
+  </si>
+  <si>
+    <t>ECE445L:MountingHole_4_40</t>
+  </si>
+  <si>
+    <t>IC1</t>
+  </si>
+  <si>
+    <t>LM4041CILPR</t>
+  </si>
+  <si>
+    <t>ti_LM4041CILPR:LM4041CILPR</t>
+  </si>
+  <si>
+    <t>ECE445L:ti_LM4041CILPR</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/general/docs/suppproductinfo.tsp?distId=26&amp;gotoUrl=https://www.ti.com/lit/gpn/lm4041a12</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>AudioJack</t>
+  </si>
+  <si>
+    <t>ECE445L:HeadphoneJack</t>
+  </si>
+  <si>
+    <t>ECE445L:Jack_3.5mm_CUI_SJ1-3523N_Horizontal</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>Header_4</t>
+  </si>
+  <si>
+    <t>ECE445L:Header_4</t>
+  </si>
+  <si>
+    <t>ECE445L:PinHeader_1x04_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>Jumper_3_Open</t>
+  </si>
+  <si>
+    <t>ECE445L:Jumper_3_Open</t>
+  </si>
+  <si>
+    <t>ECE445L:PinHeader_1x03_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>20k</t>
+  </si>
+  <si>
+    <t>Device:R</t>
+  </si>
+  <si>
+    <t>Resistor_THT:R_Axial_DIN0207_L6.3mm_D2.5mm_P10.16mm_Horizontal</t>
+  </si>
+  <si>
+    <t>R2, R5, R12</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>2k</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>47k</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>ECE445L:Potentiometer</t>
+  </si>
+  <si>
+    <t>R101</t>
+  </si>
+  <si>
+    <t>Device:R_Small</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>RESET</t>
+  </si>
+  <si>
+    <t>Switch:SW_Push</t>
+  </si>
+  <si>
+    <t>Button_Switch_THT:SW_PUSH_6mm</t>
+  </si>
+  <si>
+    <t>SW101</t>
+  </si>
+  <si>
+    <t>UP</t>
+  </si>
+  <si>
+    <t>SW102</t>
+  </si>
+  <si>
+    <t>DOWN</t>
+  </si>
+  <si>
+    <t>SW103</t>
+  </si>
+  <si>
+    <t>LEFT</t>
+  </si>
+  <si>
+    <t>SW104</t>
+  </si>
+  <si>
+    <t>RIGHT</t>
+  </si>
+  <si>
+    <t>SW105</t>
+  </si>
+  <si>
+    <t>MODE</t>
+  </si>
+  <si>
+    <t>TP1, TP2, TP3, TP4, TP5, TP6, TP7</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>ECE445L:Testpoint</t>
+  </si>
+  <si>
+    <t>ECE445L:Testpoint_1x02_P2.54mm</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>ti_TLV5616CP:TLV5616CP</t>
+  </si>
+  <si>
+    <t>ECE445L:ul_TLV5616CP</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>LM2937xMP</t>
+  </si>
+  <si>
+    <t>Regulator_Linear:LM2937xMP</t>
+  </si>
+  <si>
+    <t>ECE445L:LM2937</t>
+  </si>
+  <si>
+    <t>http://www.ti.com/lit/ds/symlink/lm2937.pdf</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>MCP34119P</t>
+  </si>
+  <si>
+    <t>ECE445L:MCP34119P</t>
+  </si>
+  <si>
+    <t>ECE445L:DIP-8_W7.62mm_LongPads</t>
+  </si>
+  <si>
+    <t>https://users.ece.utexas.edu/~valvano/Datasheets/MC34119.pdf</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Motorola</t>
+  </si>
+  <si>
+    <t>MC34119P</t>
+  </si>
+  <si>
+    <t>U101</t>
+  </si>
+  <si>
+    <t>EK-TM4C123GXL</t>
+  </si>
+  <si>
+    <t>ti_EKTM4C123GXL:EK-TM4C123GXL</t>
+  </si>
+  <si>
+    <t>ECE445L:ti_EKTM4C123GXL</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/lit/ds/symlink/tm4c123gh6pm.pdf?ts=1693244962384&amp;ref_url=https%253A%252F%252Fwww.google.com%252F</t>
+  </si>
+  <si>
+    <t>U102</t>
+  </si>
+  <si>
+    <t>ESP8266-01/ESP-01</t>
+  </si>
+  <si>
+    <t>ai_thinker_ESP8266_01:ESP8266-01/ESP-01</t>
+  </si>
+  <si>
+    <t>ECE445L:ai_thinker_ESP8266_01</t>
+  </si>
+  <si>
+    <t>https://nurdspace.nl/ESP8266</t>
+  </si>
+  <si>
+    <t>SparkFun</t>
+  </si>
+  <si>
+    <t>WRL-17146</t>
+  </si>
+  <si>
+    <t>U103</t>
+  </si>
+  <si>
+    <t>ILI9341</t>
+  </si>
+  <si>
+    <t>Hosyond</t>
+  </si>
+  <si>
+    <t>ECE445L:adafruit_st7735r</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>SD Card</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
@@ -1801,7 +2171,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1840,6 +2210,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -2251,26 +2623,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15.3" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3" customWidth="1"/>
-    <col min="2" max="3" width="11.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="46.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" style="3" customWidth="1"/>
+    <col min="2" max="3" width="11.27734375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="46.71875" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" style="3" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="23.27734375" style="3" customWidth="1"/>
     <col min="7" max="7" width="18" style="3" customWidth="1"/>
-    <col min="8" max="8" width="24.7109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="24.71875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="9.27734375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" style="2" customWidth="1"/>
     <col min="11" max="11" width="23" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="12" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -2288,7 +2660,7 @@
       </c>
       <c r="H1" s="9"/>
     </row>
-    <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="18.3" x14ac:dyDescent="0.7">
       <c r="A2" s="9" t="s">
         <v>471</v>
       </c>
@@ -2304,7 +2676,7 @@
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -2316,7 +2688,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>232</v>
       </c>
@@ -2327,7 +2699,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -2365,7 +2737,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3">
         <v>0</v>
       </c>
@@ -2398,7 +2770,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3">
         <v>0</v>
       </c>
@@ -2428,7 +2800,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3">
         <v>0</v>
       </c>
@@ -2462,7 +2834,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3">
         <v>0</v>
       </c>
@@ -2495,7 +2867,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3">
         <v>0</v>
       </c>
@@ -2531,7 +2903,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3">
         <v>0</v>
       </c>
@@ -2564,7 +2936,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3">
         <v>0</v>
       </c>
@@ -2594,7 +2966,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3">
         <v>0</v>
       </c>
@@ -2630,7 +3002,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3">
         <v>0</v>
       </c>
@@ -2660,7 +3032,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3">
         <v>0</v>
       </c>
@@ -2690,7 +3062,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3">
         <v>0</v>
       </c>
@@ -2714,7 +3086,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3">
         <v>0</v>
       </c>
@@ -2744,7 +3116,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3">
         <v>0</v>
       </c>
@@ -2774,7 +3146,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3">
         <v>0</v>
       </c>
@@ -2798,7 +3170,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3">
         <v>0</v>
       </c>
@@ -2822,7 +3194,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="3">
         <v>0</v>
       </c>
@@ -2846,7 +3218,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="3">
         <v>0</v>
       </c>
@@ -2870,7 +3242,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="3">
         <v>0</v>
       </c>
@@ -2894,7 +3266,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="3">
         <v>0</v>
       </c>
@@ -2918,7 +3290,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="3">
         <v>0</v>
       </c>
@@ -2942,7 +3314,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="3">
         <v>0</v>
       </c>
@@ -2981,7 +3353,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="3">
         <v>0</v>
       </c>
@@ -3017,7 +3389,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="3">
         <v>0</v>
       </c>
@@ -3047,7 +3419,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="3">
         <v>0</v>
       </c>
@@ -3077,7 +3449,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="3">
         <v>0</v>
       </c>
@@ -3107,7 +3479,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="3">
         <v>0</v>
       </c>
@@ -3137,7 +3509,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="3">
         <v>0</v>
       </c>
@@ -3167,7 +3539,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="3">
         <v>0</v>
       </c>
@@ -3200,7 +3572,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="3">
         <v>0</v>
       </c>
@@ -3233,7 +3605,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="3">
         <v>0</v>
       </c>
@@ -3266,7 +3638,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="3">
         <v>0</v>
       </c>
@@ -3302,7 +3674,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="3">
         <v>0</v>
       </c>
@@ -3338,7 +3710,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="3">
         <v>0</v>
       </c>
@@ -3374,7 +3746,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="3">
         <v>0</v>
       </c>
@@ -3410,7 +3782,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="3">
         <v>0</v>
       </c>
@@ -3446,7 +3818,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="3">
         <v>0</v>
       </c>
@@ -3482,7 +3854,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="3">
         <v>0</v>
       </c>
@@ -3518,7 +3890,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="3">
         <v>0</v>
       </c>
@@ -3554,7 +3926,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="3">
         <v>0</v>
       </c>
@@ -3587,7 +3959,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="3">
         <v>0</v>
       </c>
@@ -3626,7 +3998,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="3">
         <v>0</v>
       </c>
@@ -3662,7 +4034,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="3">
         <v>0</v>
       </c>
@@ -3698,7 +4070,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="3">
         <v>0</v>
       </c>
@@ -3734,7 +4106,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="3">
         <v>0</v>
       </c>
@@ -3770,7 +4142,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="3">
         <v>0</v>
       </c>
@@ -3806,7 +4178,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="3">
         <v>0</v>
       </c>
@@ -3830,7 +4202,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="3">
         <v>0</v>
       </c>
@@ -3866,7 +4238,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="3">
         <v>0</v>
       </c>
@@ -3902,7 +4274,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="3">
         <v>0</v>
       </c>
@@ -3941,7 +4313,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="3">
         <v>0</v>
       </c>
@@ -3977,7 +4349,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="3">
         <v>0</v>
       </c>
@@ -4013,7 +4385,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="3">
         <v>0</v>
       </c>
@@ -4049,7 +4421,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="3">
         <v>0</v>
       </c>
@@ -4085,7 +4457,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="3">
         <v>0</v>
       </c>
@@ -4121,7 +4493,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="3">
         <v>0</v>
       </c>
@@ -4157,7 +4529,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="3">
         <v>0</v>
       </c>
@@ -4193,7 +4565,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="3">
         <v>0</v>
       </c>
@@ -4229,7 +4601,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="3">
         <v>0</v>
       </c>
@@ -4262,7 +4634,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="3">
         <v>0</v>
       </c>
@@ -4301,7 +4673,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="3">
         <v>0</v>
       </c>
@@ -4340,7 +4712,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="3">
         <v>0</v>
       </c>
@@ -4379,7 +4751,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="3">
         <v>0</v>
       </c>
@@ -4418,7 +4790,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="3">
         <v>0</v>
       </c>
@@ -4457,7 +4829,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="3">
         <v>0</v>
       </c>
@@ -4487,7 +4859,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="3">
         <v>0</v>
       </c>
@@ -4517,7 +4889,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="3">
         <v>0</v>
       </c>
@@ -4550,7 +4922,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="3">
         <v>0</v>
       </c>
@@ -4589,7 +4961,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="3">
         <v>0</v>
       </c>
@@ -4622,7 +4994,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="3">
         <v>0</v>
       </c>
@@ -4655,7 +5027,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="3">
         <v>0</v>
       </c>
@@ -4688,7 +5060,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="3">
         <v>0</v>
       </c>
@@ -4724,7 +5096,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="3">
         <v>0</v>
       </c>
@@ -4760,7 +5132,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="3">
         <v>0</v>
       </c>
@@ -4796,7 +5168,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="3">
         <v>0</v>
       </c>
@@ -4832,7 +5204,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="3">
         <v>0</v>
       </c>
@@ -4868,7 +5240,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="3">
         <v>0</v>
       </c>
@@ -4895,7 +5267,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="3">
         <v>0</v>
       </c>
@@ -4919,7 +5291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="3">
         <v>0</v>
       </c>
@@ -4952,7 +5324,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="3">
         <v>0</v>
       </c>
@@ -4976,7 +5348,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="3">
         <v>0</v>
       </c>
@@ -5000,7 +5372,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="3">
         <v>0</v>
       </c>
@@ -5036,7 +5408,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="3">
         <v>0</v>
       </c>
@@ -5072,7 +5444,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="3">
         <v>0</v>
       </c>
@@ -5108,7 +5480,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="3">
         <v>0</v>
       </c>
@@ -5144,7 +5516,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="3">
         <v>0</v>
       </c>
@@ -5180,7 +5552,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="3">
         <v>0</v>
       </c>
@@ -5216,7 +5588,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="3">
         <v>0</v>
       </c>
@@ -5252,7 +5624,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="3">
         <v>0</v>
       </c>
@@ -5288,7 +5660,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="3">
         <v>0</v>
       </c>
@@ -5324,7 +5696,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="3">
         <v>0</v>
       </c>
@@ -5360,7 +5732,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="3">
         <v>0</v>
       </c>
@@ -5396,7 +5768,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="3">
         <v>0</v>
       </c>
@@ -5432,7 +5804,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="3">
         <v>0</v>
       </c>
@@ -5468,7 +5840,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="3">
         <v>0</v>
       </c>
@@ -5504,7 +5876,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="3">
         <v>0</v>
       </c>
@@ -5540,7 +5912,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="3">
         <v>0</v>
       </c>
@@ -5576,7 +5948,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="3">
         <v>0</v>
       </c>
@@ -5612,7 +5984,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="3">
         <v>0</v>
       </c>
@@ -5648,7 +6020,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="3">
         <v>0</v>
       </c>
@@ -5684,7 +6056,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="3">
         <v>0</v>
       </c>
@@ -5720,7 +6092,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="3">
         <v>0</v>
       </c>
@@ -5756,7 +6128,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="3">
         <v>0</v>
       </c>
@@ -5792,7 +6164,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="3">
         <v>0</v>
       </c>
@@ -5828,7 +6200,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="3">
         <v>0</v>
       </c>
@@ -5864,7 +6236,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="3">
         <v>0</v>
       </c>
@@ -5903,7 +6275,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="3">
         <v>0</v>
       </c>
@@ -5939,7 +6311,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="3">
         <v>0</v>
       </c>
@@ -5975,7 +6347,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="3">
         <v>0</v>
       </c>
@@ -6011,7 +6383,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="3">
         <v>0</v>
       </c>
@@ -6047,7 +6419,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="3">
         <v>0</v>
       </c>
@@ -6083,7 +6455,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="3">
         <v>0</v>
       </c>
@@ -6119,7 +6491,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="3">
         <v>0</v>
       </c>
@@ -6155,7 +6527,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="3">
         <v>0</v>
       </c>
@@ -6191,7 +6563,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="3">
         <v>0</v>
       </c>
@@ -6227,7 +6599,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="3">
         <v>0</v>
       </c>
@@ -6263,7 +6635,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="3">
         <v>0</v>
       </c>
@@ -6299,7 +6671,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="3">
         <v>0</v>
       </c>
@@ -6335,7 +6707,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="3">
         <v>0</v>
       </c>
@@ -6371,7 +6743,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="3">
         <v>0</v>
       </c>
@@ -6407,7 +6779,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="3">
         <v>0</v>
       </c>
@@ -6443,7 +6815,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="3">
         <v>0</v>
       </c>
@@ -6479,7 +6851,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="3">
         <v>0</v>
       </c>
@@ -6515,7 +6887,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="3">
         <v>0</v>
       </c>
@@ -6551,7 +6923,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="3">
         <v>0</v>
       </c>
@@ -6587,7 +6959,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="3">
         <v>0</v>
       </c>
@@ -6623,7 +6995,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="3">
         <v>0</v>
       </c>
@@ -6659,7 +7031,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="3">
         <v>0</v>
       </c>
@@ -6695,7 +7067,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="3">
         <v>0</v>
       </c>
@@ -6731,7 +7103,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="3">
         <v>0</v>
       </c>
@@ -6767,7 +7139,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="3">
         <v>0</v>
       </c>
@@ -6803,7 +7175,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="3">
         <v>0</v>
       </c>
@@ -6839,7 +7211,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="3">
         <v>0</v>
       </c>
@@ -6875,7 +7247,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="3">
         <v>0</v>
       </c>
@@ -6911,7 +7283,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="3">
         <v>0</v>
       </c>
@@ -6947,7 +7319,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="3">
         <v>0</v>
       </c>
@@ -6983,7 +7355,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="3">
         <v>0</v>
       </c>
@@ -7019,7 +7391,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="3">
         <v>0</v>
       </c>
@@ -7049,7 +7421,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="3">
         <v>0</v>
       </c>
@@ -7079,7 +7451,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="3">
         <v>0</v>
       </c>
@@ -7103,7 +7475,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="3">
         <v>0</v>
       </c>
@@ -7142,7 +7514,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="3">
         <v>0</v>
       </c>
@@ -7178,7 +7550,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="3">
         <v>0</v>
       </c>
@@ -7214,7 +7586,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="3">
         <v>0</v>
       </c>
@@ -7275,16 +7647,16 @@
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.6" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="4"/>
+    <col min="1" max="3" width="9.1640625" style="4"/>
     <col min="4" max="4" width="28" style="4" customWidth="1"/>
-    <col min="5" max="10" width="9.140625" style="4"/>
-    <col min="11" max="11" width="16.140625" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="4"/>
+    <col min="5" max="10" width="9.1640625" style="4"/>
+    <col min="11" max="11" width="16.1640625" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -7322,7 +7694,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="5">
         <v>0</v>
       </c>
@@ -7351,7 +7723,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="5">
         <v>0</v>
       </c>
@@ -7380,7 +7752,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="5">
         <v>0</v>
       </c>
@@ -7409,7 +7781,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="5">
         <v>0</v>
       </c>
@@ -7438,7 +7810,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="5">
         <v>0</v>
       </c>
@@ -7467,7 +7839,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="5">
         <v>0</v>
       </c>
@@ -7491,7 +7863,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="5">
         <v>0</v>
       </c>
@@ -7525,139 +7897,990 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="A1:E18"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="1"/>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>511</v>
+      </c>
+      <c r="B1" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>513</v>
+      </c>
+      <c r="B2" s="16">
+        <v>45379.731944444444</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>514</v>
+      </c>
+      <c r="B3" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>516</v>
+      </c>
+      <c r="B4" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>518</v>
+      </c>
+      <c r="B5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>520</v>
+      </c>
+      <c r="B9" t="s">
+        <v>521</v>
+      </c>
+      <c r="C9" t="s">
+        <v>522</v>
+      </c>
+      <c r="D9" t="s">
+        <v>523</v>
+      </c>
+      <c r="E9" t="s">
+        <v>524</v>
+      </c>
+      <c r="F9" t="s">
+        <v>525</v>
+      </c>
+      <c r="G9" t="s">
+        <v>526</v>
+      </c>
+      <c r="H9" t="s">
+        <v>527</v>
+      </c>
+      <c r="I9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" t="s">
+        <v>528</v>
+      </c>
+      <c r="L9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>529</v>
+      </c>
+      <c r="D10" t="s">
+        <v>530</v>
+      </c>
+      <c r="E10" t="s">
+        <v>531</v>
+      </c>
+      <c r="F10" t="s">
+        <v>532</v>
+      </c>
+      <c r="G10" t="s">
+        <v>533</v>
+      </c>
+      <c r="H10" t="s">
+        <v>534</v>
+      </c>
+      <c r="I10" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>535</v>
+      </c>
+      <c r="D11" t="s">
+        <v>536</v>
+      </c>
+      <c r="E11" t="s">
+        <v>537</v>
+      </c>
+      <c r="F11" t="s">
+        <v>532</v>
+      </c>
+      <c r="G11" t="s">
+        <v>533</v>
+      </c>
+      <c r="H11" t="s">
+        <v>534</v>
+      </c>
+      <c r="I11" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>538</v>
+      </c>
+      <c r="D12" t="s">
+        <v>539</v>
+      </c>
+      <c r="E12" t="s">
+        <v>531</v>
+      </c>
+      <c r="F12" t="s">
+        <v>532</v>
+      </c>
+      <c r="G12" t="s">
+        <v>533</v>
+      </c>
+      <c r="H12" t="s">
+        <v>534</v>
+      </c>
+      <c r="I12" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>540</v>
+      </c>
+      <c r="D13" t="s">
+        <v>541</v>
+      </c>
+      <c r="E13" t="s">
+        <v>542</v>
+      </c>
+      <c r="F13" t="s">
+        <v>532</v>
+      </c>
+      <c r="G13" t="s">
+        <v>533</v>
+      </c>
+      <c r="H13" t="s">
+        <v>534</v>
+      </c>
+      <c r="I13" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>543</v>
+      </c>
+      <c r="D14" t="s">
+        <v>539</v>
+      </c>
+      <c r="E14" t="s">
+        <v>544</v>
+      </c>
+      <c r="F14" t="s">
+        <v>545</v>
+      </c>
+      <c r="G14" t="s">
+        <v>533</v>
+      </c>
+      <c r="H14" t="s">
+        <v>534</v>
+      </c>
+      <c r="I14" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A15">
+        <v>6</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>546</v>
+      </c>
+      <c r="D15" t="s">
+        <v>533</v>
+      </c>
+      <c r="E15" t="s">
+        <v>547</v>
+      </c>
+      <c r="F15" t="s">
+        <v>548</v>
+      </c>
+      <c r="H15" t="s">
+        <v>534</v>
+      </c>
+      <c r="I15" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A16">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>549</v>
+      </c>
+      <c r="D16" t="s">
+        <v>550</v>
+      </c>
+      <c r="E16" t="s">
+        <v>551</v>
+      </c>
+      <c r="F16" t="s">
+        <v>552</v>
+      </c>
+      <c r="G16" t="s">
+        <v>553</v>
+      </c>
+      <c r="H16" t="s">
+        <v>534</v>
+      </c>
+      <c r="I16" s="17">
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>554</v>
+      </c>
+      <c r="K16" t="s">
+        <v>555</v>
+      </c>
+      <c r="L16" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A17">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>556</v>
+      </c>
+      <c r="D17" t="s">
+        <v>557</v>
+      </c>
+      <c r="E17" t="s">
+        <v>558</v>
+      </c>
+      <c r="F17" t="s">
+        <v>559</v>
+      </c>
+      <c r="G17" t="s">
+        <v>533</v>
+      </c>
+      <c r="H17" t="s">
+        <v>534</v>
+      </c>
+      <c r="I17" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A18">
+        <v>9</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>560</v>
+      </c>
+      <c r="D18" t="s">
+        <v>561</v>
+      </c>
+      <c r="E18" t="s">
+        <v>562</v>
+      </c>
+      <c r="F18" t="s">
+        <v>563</v>
+      </c>
+      <c r="G18" t="s">
+        <v>533</v>
+      </c>
+      <c r="H18" t="s">
+        <v>534</v>
+      </c>
+      <c r="I18" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A19">
+        <v>10</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>564</v>
+      </c>
+      <c r="D19" t="s">
+        <v>565</v>
+      </c>
+      <c r="E19" t="s">
+        <v>566</v>
+      </c>
+      <c r="F19" t="s">
+        <v>567</v>
+      </c>
+      <c r="G19" t="s">
+        <v>533</v>
+      </c>
+      <c r="H19" t="s">
+        <v>534</v>
+      </c>
+      <c r="I19" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A20">
+        <v>11</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>568</v>
+      </c>
+      <c r="D20" t="s">
+        <v>569</v>
+      </c>
+      <c r="E20" t="s">
+        <v>570</v>
+      </c>
+      <c r="F20" t="s">
+        <v>571</v>
+      </c>
+      <c r="G20" t="s">
+        <v>533</v>
+      </c>
+      <c r="H20" t="s">
+        <v>534</v>
+      </c>
+      <c r="I20" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A21">
+        <v>12</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>572</v>
+      </c>
+      <c r="D21" t="s">
+        <v>573</v>
+      </c>
+      <c r="E21" t="s">
+        <v>570</v>
+      </c>
+      <c r="F21" t="s">
+        <v>571</v>
+      </c>
+      <c r="G21" t="s">
+        <v>533</v>
+      </c>
+      <c r="H21" t="s">
+        <v>534</v>
+      </c>
+      <c r="I21" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A22">
+        <v>13</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>574</v>
+      </c>
+      <c r="D22" t="s">
+        <v>575</v>
+      </c>
+      <c r="E22" t="s">
+        <v>570</v>
+      </c>
+      <c r="F22" t="s">
+        <v>571</v>
+      </c>
+      <c r="G22" t="s">
+        <v>533</v>
+      </c>
+      <c r="H22" t="s">
+        <v>534</v>
+      </c>
+      <c r="I22" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A23">
+        <v>14</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>576</v>
+      </c>
+      <c r="D23" t="s">
+        <v>577</v>
+      </c>
+      <c r="E23" t="s">
+        <v>570</v>
+      </c>
+      <c r="F23" t="s">
+        <v>571</v>
+      </c>
+      <c r="G23" t="s">
+        <v>533</v>
+      </c>
+      <c r="H23" t="s">
+        <v>534</v>
+      </c>
+      <c r="I23" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A24">
+        <v>15</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>578</v>
+      </c>
+      <c r="D24" t="s">
+        <v>573</v>
+      </c>
+      <c r="E24" t="s">
+        <v>579</v>
+      </c>
+      <c r="F24" t="s">
+        <v>579</v>
+      </c>
+      <c r="H24" t="s">
+        <v>534</v>
+      </c>
+      <c r="I24" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A25">
+        <v>16</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>580</v>
+      </c>
+      <c r="D25" t="s">
+        <v>573</v>
+      </c>
+      <c r="E25" t="s">
+        <v>581</v>
+      </c>
+      <c r="F25" t="s">
+        <v>571</v>
+      </c>
+      <c r="G25" t="s">
+        <v>533</v>
+      </c>
+      <c r="H25" t="s">
+        <v>534</v>
+      </c>
+      <c r="I25" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A26">
+        <v>17</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>582</v>
+      </c>
+      <c r="D26" t="s">
+        <v>583</v>
+      </c>
+      <c r="E26" t="s">
+        <v>584</v>
+      </c>
+      <c r="F26" t="s">
+        <v>585</v>
+      </c>
+      <c r="G26" t="s">
+        <v>533</v>
+      </c>
+      <c r="H26" t="s">
+        <v>534</v>
+      </c>
+      <c r="I26" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A27">
+        <v>18</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>586</v>
+      </c>
+      <c r="D27" t="s">
+        <v>587</v>
+      </c>
+      <c r="E27" t="s">
+        <v>584</v>
+      </c>
+      <c r="F27" t="s">
+        <v>585</v>
+      </c>
+      <c r="G27" t="s">
+        <v>533</v>
+      </c>
+      <c r="H27" t="s">
+        <v>534</v>
+      </c>
+      <c r="I27" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A28">
+        <v>19</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>588</v>
+      </c>
+      <c r="D28" t="s">
+        <v>589</v>
+      </c>
+      <c r="E28" t="s">
+        <v>584</v>
+      </c>
+      <c r="F28" t="s">
+        <v>585</v>
+      </c>
+      <c r="G28" t="s">
+        <v>533</v>
+      </c>
+      <c r="H28" t="s">
+        <v>534</v>
+      </c>
+      <c r="I28" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A29">
+        <v>20</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>590</v>
+      </c>
+      <c r="D29" t="s">
+        <v>591</v>
+      </c>
+      <c r="E29" t="s">
+        <v>584</v>
+      </c>
+      <c r="F29" t="s">
+        <v>585</v>
+      </c>
+      <c r="G29" t="s">
+        <v>533</v>
+      </c>
+      <c r="H29" t="s">
+        <v>534</v>
+      </c>
+      <c r="I29" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A30">
+        <v>21</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>592</v>
+      </c>
+      <c r="D30" t="s">
+        <v>593</v>
+      </c>
+      <c r="E30" t="s">
+        <v>584</v>
+      </c>
+      <c r="F30" t="s">
+        <v>585</v>
+      </c>
+      <c r="G30" t="s">
+        <v>533</v>
+      </c>
+      <c r="H30" t="s">
+        <v>534</v>
+      </c>
+      <c r="I30" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A31">
+        <v>22</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>594</v>
+      </c>
+      <c r="D31" t="s">
+        <v>595</v>
+      </c>
+      <c r="E31" t="s">
+        <v>584</v>
+      </c>
+      <c r="F31" t="s">
+        <v>585</v>
+      </c>
+      <c r="G31" t="s">
+        <v>533</v>
+      </c>
+      <c r="H31" t="s">
+        <v>534</v>
+      </c>
+      <c r="I31" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A32">
+        <v>23</v>
+      </c>
+      <c r="B32">
+        <v>7</v>
+      </c>
+      <c r="C32" t="s">
+        <v>596</v>
+      </c>
+      <c r="D32" t="s">
+        <v>597</v>
+      </c>
+      <c r="E32" t="s">
+        <v>598</v>
+      </c>
+      <c r="F32" t="s">
+        <v>599</v>
+      </c>
+      <c r="G32" t="s">
+        <v>533</v>
+      </c>
+      <c r="H32" t="s">
+        <v>534</v>
+      </c>
+      <c r="I32" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A33">
+        <v>24</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>600</v>
+      </c>
+      <c r="D33" t="s">
+        <v>490</v>
+      </c>
+      <c r="E33" t="s">
+        <v>601</v>
+      </c>
+      <c r="F33" t="s">
+        <v>602</v>
+      </c>
+      <c r="G33" t="s">
+        <v>490</v>
+      </c>
+      <c r="H33" t="s">
+        <v>534</v>
+      </c>
+      <c r="I33" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A34">
+        <v>25</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>603</v>
+      </c>
+      <c r="D34" t="s">
+        <v>604</v>
+      </c>
+      <c r="E34" t="s">
+        <v>605</v>
+      </c>
+      <c r="F34" t="s">
+        <v>606</v>
+      </c>
+      <c r="G34" t="s">
+        <v>607</v>
+      </c>
+      <c r="H34" t="s">
+        <v>534</v>
+      </c>
+      <c r="I34" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A35">
+        <v>26</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>608</v>
+      </c>
+      <c r="D35" t="s">
+        <v>609</v>
+      </c>
+      <c r="E35" t="s">
+        <v>610</v>
+      </c>
+      <c r="F35" t="s">
+        <v>611</v>
+      </c>
+      <c r="G35" t="s">
+        <v>612</v>
+      </c>
+      <c r="H35" t="s">
+        <v>534</v>
+      </c>
+      <c r="I35" s="17">
+        <v>0</v>
+      </c>
+      <c r="J35" t="s">
+        <v>613</v>
+      </c>
+      <c r="K35" t="s">
+        <v>614</v>
+      </c>
+      <c r="L35" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A36">
+        <v>27</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>616</v>
+      </c>
+      <c r="D36" t="s">
+        <v>617</v>
+      </c>
+      <c r="E36" t="s">
+        <v>618</v>
+      </c>
+      <c r="F36" t="s">
+        <v>619</v>
+      </c>
+      <c r="G36" t="s">
+        <v>620</v>
+      </c>
+      <c r="H36" t="s">
+        <v>534</v>
+      </c>
+      <c r="I36" s="17">
+        <v>0</v>
+      </c>
+      <c r="J36" t="s">
+        <v>554</v>
+      </c>
+      <c r="K36" t="s">
+        <v>555</v>
+      </c>
+      <c r="L36" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A37">
+        <v>28</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>621</v>
+      </c>
+      <c r="D37" t="s">
+        <v>622</v>
+      </c>
+      <c r="E37" t="s">
+        <v>623</v>
+      </c>
+      <c r="F37" t="s">
+        <v>624</v>
+      </c>
+      <c r="G37" t="s">
+        <v>625</v>
+      </c>
+      <c r="H37" t="s">
+        <v>534</v>
+      </c>
+      <c r="I37" s="17">
+        <v>0</v>
+      </c>
+      <c r="J37" t="s">
+        <v>554</v>
+      </c>
+      <c r="K37" t="s">
+        <v>626</v>
+      </c>
+      <c r="L37" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A38">
+        <v>29</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>628</v>
+      </c>
+      <c r="D38" t="s">
+        <v>629</v>
+      </c>
+      <c r="E38" t="s">
+        <v>630</v>
+      </c>
+      <c r="F38" t="s">
+        <v>631</v>
+      </c>
+      <c r="H38" t="s">
+        <v>632</v>
+      </c>
+      <c r="I38" s="17">
+        <v>15</v>
+      </c>
+      <c r="J38" t="s">
+        <v>554</v>
+      </c>
+      <c r="K38" t="s">
+        <v>338</v>
+      </c>
+      <c r="L38">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>633</v>
+      </c>
+      <c r="D39" t="s">
+        <v>633</v>
+      </c>
+      <c r="H39" t="s">
+        <v>632</v>
+      </c>
+      <c r="I39" s="17">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>